<commit_message>
minor changes (docstrings, error handling), and adding material for 1_sut default model.
</commit_message>
<xml_diff>
--- a/default/1_sut/concept.xlsx
+++ b/default/1_sut/concept.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\1_sut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53251CC-D5CB-4D44-A1D2-46019DB4ADD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD58E0C2-2671-4FAC-874D-6152EBEF98A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="concept" sheetId="2" r:id="rId1"/>
@@ -258,7 +258,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0;\-0;\-"/>
-    <numFmt numFmtId="165" formatCode="0.00;\-0.00;\-"/>
+    <numFmt numFmtId="165" formatCode="0.000;\-0.000;\-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -358,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -368,13 +368,20 @@
       <alignment textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,17 +665,19 @@
   <dimension ref="A1:AB42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R13" sqref="R13"/>
+      <selection pane="bottomRight" activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="8.7265625" style="1"/>
     <col min="4" max="4" width="13.26953125" style="1" customWidth="1"/>
-    <col min="5" max="32" width="4.7265625" style="1" customWidth="1"/>
+    <col min="5" max="17" width="4.7265625" style="1" customWidth="1"/>
+    <col min="18" max="28" width="5.6328125" style="11" customWidth="1"/>
+    <col min="29" max="32" width="4.7265625" style="1" customWidth="1"/>
     <col min="33" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
@@ -685,13 +694,13 @@
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
@@ -711,22 +720,22 @@
       <c r="M2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AA2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AB2" s="11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -764,32 +773,33 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3" t="s">
+      <c r="U3" s="12"/>
+      <c r="V3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="W3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="X3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AA3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AB3" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -811,10 +821,10 @@
       <c r="O5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="Z5" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -844,24 +854,24 @@
         <f>SUM(I6:K6,M6)</f>
         <v>110</v>
       </c>
-      <c r="V6" s="5">
+      <c r="V6" s="10">
         <f t="array" ref="V6:X8">MMULT(I6:K8,MINVERSE(O10:O12*_xlfn.MUNIT(3)))</f>
         <v>0</v>
       </c>
-      <c r="W6" s="5">
-        <v>0</v>
-      </c>
-      <c r="X6" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="5">
+      <c r="W6" s="10">
+        <v>0</v>
+      </c>
+      <c r="X6" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="10">
         <f t="array" ref="Z6:AB8">MMULT(TRANSPOSE(E10:G12),MINVERSE(O10:O12*_xlfn.MUNIT(3)))</f>
         <v>0.90909090909090906</v>
       </c>
-      <c r="AA6" s="5">
+      <c r="AA6" s="10">
         <v>0.16666666666666666</v>
       </c>
-      <c r="AB6" s="5">
+      <c r="AB6" s="10">
         <v>0</v>
       </c>
     </row>
@@ -891,22 +901,22 @@
         <f>SUM(I7:K7,M7)</f>
         <v>50</v>
       </c>
-      <c r="V7" s="5">
+      <c r="V7" s="10">
         <v>0.27272727272727271</v>
       </c>
-      <c r="W7" s="5">
-        <v>0</v>
-      </c>
-      <c r="X7" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="5">
+      <c r="W7" s="10">
+        <v>0</v>
+      </c>
+      <c r="X7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="10">
         <v>0.83333333333333337</v>
       </c>
-      <c r="AB7" s="5">
+      <c r="AB7" s="10">
         <v>0</v>
       </c>
     </row>
@@ -936,25 +946,25 @@
         <f>SUM(I8:K8,M8)</f>
         <v>30</v>
       </c>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="V8" s="5">
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="V8" s="10">
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="W8" s="5">
-        <v>0</v>
-      </c>
-      <c r="X8" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="5">
+      <c r="W8" s="10">
+        <v>0</v>
+      </c>
+      <c r="X8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="10">
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="AA8" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="5">
+      <c r="AA8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="10">
         <v>1</v>
       </c>
     </row>
@@ -965,7 +975,7 @@
       <c r="O9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="R9" s="11" t="s">
         <v>29</v>
       </c>
     </row>
@@ -989,14 +999,14 @@
         <f>SUM(E10:G10)</f>
         <v>110</v>
       </c>
-      <c r="R10" s="5">
+      <c r="R10" s="10">
         <f t="array" ref="R10:T12">MMULT(E10:G12,MINVERSE(O6:O8*_xlfn.MUNIT(3)))</f>
         <v>0.90909090909090906</v>
       </c>
-      <c r="S10" s="5">
-        <v>0</v>
-      </c>
-      <c r="T10" s="5">
+      <c r="S10" s="10">
+        <v>0</v>
+      </c>
+      <c r="T10" s="10">
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -1020,13 +1030,13 @@
         <f t="shared" ref="O11:O12" si="0">SUM(E11:G11)</f>
         <v>60</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11" s="10">
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="S11" s="5">
+      <c r="S11" s="10">
         <v>1</v>
       </c>
-      <c r="T11" s="5">
+      <c r="T11" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1050,13 +1060,13 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="R12" s="5">
-        <v>0</v>
-      </c>
-      <c r="S12" s="5">
-        <v>0</v>
-      </c>
-      <c r="T12" s="5">
+      <c r="R12" s="10">
+        <v>0</v>
+      </c>
+      <c r="S12" s="10">
+        <v>0</v>
+      </c>
+      <c r="T12" s="10">
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -1064,7 +1074,7 @@
       <c r="I13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="V13" s="11" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1087,14 +1097,14 @@
       <c r="K14" s="4">
         <v>6</v>
       </c>
-      <c r="V14" s="5">
+      <c r="V14" s="10">
         <f t="array" ref="V14:X14">MMULT(I14:K14,MINVERSE(O10:O12*_xlfn.MUNIT(3)))</f>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="W14" s="5">
+      <c r="W14" s="10">
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="X14" s="5">
+      <c r="X14" s="10">
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -1135,10 +1145,10 @@
       <c r="Q20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="U20" s="1" t="s">
+      <c r="U20" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="V20" s="1" t="s">
+      <c r="V20" s="11" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1152,33 +1162,33 @@
       <c r="D21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="5">
         <f t="array" ref="I21:K23">MMULT(V6:X8,O25:O27*_xlfn.MUNIT(3))</f>
         <v>0</v>
       </c>
-      <c r="J21" s="7">
-        <v>0</v>
-      </c>
-      <c r="K21" s="7">
+      <c r="J21" s="5">
+        <v>0</v>
+      </c>
+      <c r="K21" s="5">
         <v>0</v>
       </c>
       <c r="M21" s="4">
         <v>110</v>
       </c>
-      <c r="O21" s="8">
+      <c r="O21" s="6">
         <v>110</v>
       </c>
-      <c r="Q21" s="9">
+      <c r="Q21" s="7">
         <f t="array" ref="Q21:Q23">O21:O23-MMULT(V6:X8,O25:O27)-M21:M23</f>
         <v>0</v>
       </c>
-      <c r="U21" s="1" t="s">
+      <c r="U21" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="V21" s="1" t="s">
+      <c r="V21" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="Y21" s="1" t="s">
+      <c r="Y21" s="11" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1192,28 +1202,28 @@
       <c r="D22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="5">
         <v>29.999999999999996</v>
       </c>
-      <c r="J22" s="7">
-        <v>0</v>
-      </c>
-      <c r="K22" s="7">
+      <c r="J22" s="5">
+        <v>0</v>
+      </c>
+      <c r="K22" s="5">
         <v>0</v>
       </c>
       <c r="M22" s="4">
         <v>20</v>
       </c>
-      <c r="O22" s="8">
+      <c r="O22" s="6">
         <v>50</v>
       </c>
-      <c r="Q22" s="10">
-        <v>0</v>
-      </c>
-      <c r="V22" s="1" t="s">
+      <c r="Q22" s="8">
+        <v>0</v>
+      </c>
+      <c r="V22" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="Y22" s="1" t="s">
+      <c r="Y22" s="11" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1227,28 +1237,28 @@
       <c r="D23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="5">
         <v>10</v>
       </c>
-      <c r="J23" s="7">
-        <v>0</v>
-      </c>
-      <c r="K23" s="7">
+      <c r="J23" s="5">
+        <v>0</v>
+      </c>
+      <c r="K23" s="5">
         <v>0</v>
       </c>
       <c r="M23" s="4">
         <v>20</v>
       </c>
-      <c r="O23" s="8">
+      <c r="O23" s="6">
         <v>30</v>
       </c>
-      <c r="Q23" s="11">
-        <v>0</v>
-      </c>
-      <c r="V23" s="1" t="s">
+      <c r="Q23" s="9">
+        <v>0</v>
+      </c>
+      <c r="V23" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Y23" s="1" t="s">
+      <c r="Y23" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1262,10 +1272,10 @@
       <c r="Q24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V24" s="1" t="s">
+      <c r="V24" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="Y24" s="1" t="s">
+      <c r="Y24" s="11" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1276,20 +1286,20 @@
       <c r="D25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="5">
         <f t="array" ref="E25:G27">MMULT(R10:T12,O21:O23*_xlfn.MUNIT(3))</f>
         <v>100</v>
       </c>
-      <c r="F25" s="7">
-        <v>0</v>
-      </c>
-      <c r="G25" s="7">
+      <c r="F25" s="5">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5">
         <v>10</v>
       </c>
-      <c r="O25" s="8">
+      <c r="O25" s="6">
         <v>110</v>
       </c>
-      <c r="Q25" s="9">
+      <c r="Q25" s="7">
         <f t="array" ref="Q25:Q27">O25:O27-MMULT(R10:T12,O21:O23)</f>
         <v>0</v>
       </c>
@@ -1301,19 +1311,19 @@
       <c r="D26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="5">
         <v>10</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="5">
         <v>50</v>
       </c>
-      <c r="G26" s="7">
-        <v>0</v>
-      </c>
-      <c r="O26" s="8">
+      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+      <c r="O26" s="6">
         <v>60</v>
       </c>
-      <c r="Q26" s="10">
+      <c r="Q26" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1324,19 +1334,19 @@
       <c r="D27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="7">
-        <v>0</v>
-      </c>
-      <c r="F27" s="7">
-        <v>0</v>
-      </c>
-      <c r="G27" s="7">
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
         <v>20</v>
       </c>
-      <c r="O27" s="8">
+      <c r="O27" s="6">
         <v>20</v>
       </c>
-      <c r="Q27" s="11">
+      <c r="Q27" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1355,14 +1365,14 @@
       <c r="D29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="5">
         <f t="array" ref="I29:K29">MMULT(V14:X14,O25:O27*_xlfn.MUNIT(3))</f>
         <v>10</v>
       </c>
-      <c r="J29" s="7">
+      <c r="J29" s="5">
         <v>4</v>
       </c>
-      <c r="K29" s="7">
+      <c r="K29" s="5">
         <v>6.0000000000000009</v>
       </c>
     </row>
@@ -1384,10 +1394,10 @@
       <c r="Q33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="U33" s="1" t="s">
+      <c r="U33" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="V33" s="1" t="s">
+      <c r="V33" s="11" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1401,34 +1411,34 @@
       <c r="D34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I34" s="7">
+      <c r="I34" s="5">
         <f t="array" ref="I34:K36">MMULT(V6:X8,O38:O40*_xlfn.MUNIT(3))</f>
         <v>0</v>
       </c>
-      <c r="J34" s="7">
-        <v>0</v>
-      </c>
-      <c r="K34" s="7">
+      <c r="J34" s="5">
+        <v>0</v>
+      </c>
+      <c r="K34" s="5">
         <v>0</v>
       </c>
       <c r="M34" s="4">
         <f t="array" ref="M34:M36">M21:M23</f>
         <v>110</v>
       </c>
-      <c r="O34" s="8">
+      <c r="O34" s="6">
         <v>110</v>
       </c>
-      <c r="Q34" s="9">
+      <c r="Q34" s="7">
         <f t="array" ref="Q34:Q36">O34:O36-MMULT(V6:X8,O38:O40)-M34:M36</f>
         <v>0</v>
       </c>
-      <c r="U34" s="1" t="s">
+      <c r="U34" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="V34" s="1" t="s">
+      <c r="V34" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="Y34" s="1" t="s">
+      <c r="Y34" s="11" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1442,28 +1452,28 @@
       <c r="D35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="7">
+      <c r="I35" s="5">
         <v>29.999999999999996</v>
       </c>
-      <c r="J35" s="7">
-        <v>0</v>
-      </c>
-      <c r="K35" s="7">
+      <c r="J35" s="5">
+        <v>0</v>
+      </c>
+      <c r="K35" s="5">
         <v>0</v>
       </c>
       <c r="M35" s="4">
         <v>20</v>
       </c>
-      <c r="O35" s="8">
+      <c r="O35" s="6">
         <v>50</v>
       </c>
-      <c r="Q35" s="10">
-        <v>0</v>
-      </c>
-      <c r="V35" s="1" t="s">
+      <c r="Q35" s="8">
+        <v>0</v>
+      </c>
+      <c r="V35" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="Y35" s="1" t="s">
+      <c r="Y35" s="11" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1477,28 +1487,28 @@
       <c r="D36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I36" s="7">
+      <c r="I36" s="5">
         <v>10</v>
       </c>
-      <c r="J36" s="7">
-        <v>0</v>
-      </c>
-      <c r="K36" s="7">
+      <c r="J36" s="5">
+        <v>0</v>
+      </c>
+      <c r="K36" s="5">
         <v>0</v>
       </c>
       <c r="M36" s="4">
         <v>20</v>
       </c>
-      <c r="O36" s="8">
+      <c r="O36" s="6">
         <v>30</v>
       </c>
-      <c r="Q36" s="11">
-        <v>0</v>
-      </c>
-      <c r="V36" s="1" t="s">
+      <c r="Q36" s="9">
+        <v>0</v>
+      </c>
+      <c r="V36" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Y36" s="1" t="s">
+      <c r="Y36" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1512,10 +1522,10 @@
       <c r="Q37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="V37" s="1" t="s">
+      <c r="V37" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="Y37" s="1" t="s">
+      <c r="Y37" s="11" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1526,20 +1536,20 @@
       <c r="D38" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="5">
         <f t="array" ref="E38:G40">TRANSPOSE(MMULT(Z6:AB8,O38:O40*_xlfn.MUNIT(3)))</f>
         <v>100</v>
       </c>
-      <c r="F38" s="7">
-        <v>0</v>
-      </c>
-      <c r="G38" s="7">
+      <c r="F38" s="5">
+        <v>0</v>
+      </c>
+      <c r="G38" s="5">
         <v>10</v>
       </c>
-      <c r="O38" s="8">
+      <c r="O38" s="6">
         <v>110</v>
       </c>
-      <c r="Q38" s="9">
+      <c r="Q38" s="7">
         <f t="array" ref="Q38:Q40">O34:O36-MMULT(Z6:AB8,O38:O40)</f>
         <v>0</v>
       </c>
@@ -1551,19 +1561,19 @@
       <c r="D39" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="5">
         <v>10</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="5">
         <v>50</v>
       </c>
-      <c r="G39" s="7">
-        <v>0</v>
-      </c>
-      <c r="O39" s="8">
+      <c r="G39" s="5">
+        <v>0</v>
+      </c>
+      <c r="O39" s="6">
         <v>60</v>
       </c>
-      <c r="Q39" s="10">
+      <c r="Q39" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1574,19 +1584,19 @@
       <c r="D40" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="7">
-        <v>0</v>
-      </c>
-      <c r="F40" s="7">
-        <v>0</v>
-      </c>
-      <c r="G40" s="7">
+      <c r="E40" s="5">
+        <v>0</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0</v>
+      </c>
+      <c r="G40" s="5">
         <v>20</v>
       </c>
-      <c r="O40" s="8">
+      <c r="O40" s="6">
         <v>20</v>
       </c>
-      <c r="Q40" s="11">
+      <c r="Q40" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1605,14 +1615,14 @@
       <c r="D42" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I42" s="7">
+      <c r="I42" s="5">
         <f t="array" ref="I42:K42">MMULT(V14:X14,O38:O40*_xlfn.MUNIT(3))</f>
         <v>10</v>
       </c>
-      <c r="J42" s="7">
+      <c r="J42" s="5">
         <v>4</v>
       </c>
-      <c r="K42" s="7">
+      <c r="K42" s="5">
         <v>6.0000000000000009</v>
       </c>
     </row>

</xml_diff>